<commit_message>
"add tracking in exported excel"
</commit_message>
<xml_diff>
--- a/netforce_account_report/netforce_account_report/reports/account_gl_detail.xlsx
+++ b/netforce_account_report/netforce_account_report/reports/account_gl_detail.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>General Ledger [Details]</t>
   </si>
@@ -24,6 +24,21 @@
   </si>
   <si>
     <t>From {{fmt_date date_from}} to {{fmt_date date_to}}</t>
+  </si>
+  <si>
+    <t>{{#if track_name}}</t>
+  </si>
+  <si>
+    <t>Tracking: {{track_name}}</t>
+  </si>
+  <si>
+    <t>{{/if}}</t>
+  </si>
+  <si>
+    <t>{{#if track2_name}}</t>
+  </si>
+  <si>
+    <t>Tracking2: {{track2_name}}</t>
   </si>
   <si>
     <t>Account Code</t>
@@ -293,10 +308,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -366,120 +381,198 @@
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
     </row>
-    <row r="5" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="s">
+    <row r="5" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="B11" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="C11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="D11" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="F11" s="7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+      <c r="G11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="H11" s="7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="0" t="s">
+      <c r="I11" s="7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="0" t="s">
+      <c r="J11" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="0" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="0" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="J13" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="0" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="0" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="C15" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="10" t="s">
+      <c r="D15" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="E15" s="0" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="s">
+      <c r="F15" s="0" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H12" s="11" t="s">
+      <c r="G15" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="H15" s="10" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>26</v>
+      <c r="I15" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="H17" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="9">
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="C10:E10"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
IMP:Add Tax No. In Report Gl Detail
</commit_message>
<xml_diff>
--- a/netforce_account_report/netforce_account_report/reports/account_gl_detail.xlsx
+++ b/netforce_account_report/netforce_account_report/reports/account_gl_detail.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>General Ledger [Details]</t>
   </si>
@@ -50,6 +50,9 @@
     <t>Number</t>
   </si>
   <si>
+    <t>Tax No.</t>
+  </si>
+  <si>
     <t>Description</t>
   </si>
   <si>
@@ -90,6 +93,9 @@
   </si>
   <si>
     <t>{{number}}</t>
+  </si>
+  <si>
+    <t>{{tax_no}}</t>
   </si>
   <si>
     <t>{{description}}</t>
@@ -314,10 +320,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -325,13 +331,14 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="34.4387755102041"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4948979591837"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="38.6173469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.4540816326531"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="0" width="17.5918367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.3928571428571"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="20.6020408163265"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.95408163265306"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.6938775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="38.6173469387755"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.4540816326531"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="17.5918367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.3928571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.6020408163265"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="8.95408163265306"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -346,6 +353,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1"/>
@@ -357,10 +365,11 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="1"/>
+      <c r="H2" s="3"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
@@ -372,10 +381,11 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="1"/>
+      <c r="H3" s="3"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
     </row>
     <row r="4" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="4"/>
@@ -387,10 +397,11 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
-      <c r="H4" s="4"/>
+      <c r="H4" s="5"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
@@ -402,10 +413,11 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
-      <c r="H5" s="4"/>
+      <c r="H5" s="5"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="4"/>
@@ -417,10 +429,11 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
-      <c r="H6" s="4"/>
+      <c r="H6" s="5"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="5" t="s">
@@ -432,10 +445,11 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
-      <c r="H7" s="4"/>
+      <c r="H7" s="5"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
@@ -447,10 +461,11 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="4"/>
+      <c r="H8" s="5"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="4"/>
@@ -462,10 +477,11 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
-      <c r="H9" s="4"/>
+      <c r="H9" s="5"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
     </row>
     <row r="10" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
@@ -475,12 +491,13 @@
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
-      <c r="F10" s="1"/>
+      <c r="F10" s="5"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="s">
@@ -516,86 +533,92 @@
       <c r="K11" s="7" t="s">
         <v>18</v>
       </c>
+      <c r="L11" s="7" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="J13" s="9" t="s">
         <v>21</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B15" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="H15" s="10" t="s">
         <v>29</v>
       </c>
+      <c r="H15" s="0" t="s">
+        <v>30</v>
+      </c>
       <c r="I15" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K15" s="10" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="L15" s="10" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B16" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H17" s="11" t="s">
-        <v>34</v>
-      </c>
       <c r="I17" s="11" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
FIX:Edit Report Gl Detail
</commit_message>
<xml_diff>
--- a/netforce_account_report/netforce_account_report/reports/account_gl_detail.xlsx
+++ b/netforce_account_report/netforce_account_report/reports/account_gl_detail.xlsx
@@ -59,7 +59,7 @@
     <t>Contact</t>
   </si>
   <si>
-    <t>Track</t>
+    <t>Track-1</t>
   </si>
   <si>
     <t>Track-2</t>
@@ -323,7 +323,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>